<commit_message>
01-A: added Turner prior to BHM case study. 02-B: updated decision model inputs and PSA.
</commit_message>
<xml_diff>
--- a/data/Larotrectinib-ORR.xlsx
+++ b/data/Larotrectinib-ORR.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12770" windowHeight="4080" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12770" windowHeight="4080" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
     <sheet name="EPAR" sheetId="1" r:id="rId2"/>
     <sheet name="ERG-Table7" sheetId="3" r:id="rId3"/>
+    <sheet name="compare" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="31">
   <si>
     <t>Tumour type</t>
   </si>
@@ -113,13 +114,19 @@
   </si>
   <si>
     <t>Data as given in Table 7 from ERG report (p. 66) in NICE committee papers (p. 490 in pdf file).</t>
+  </si>
+  <si>
+    <t>Comare</t>
+  </si>
+  <si>
+    <t>ERG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +138,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -156,9 +170,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,7 +499,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -678,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -856,4 +873,349 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="30.26953125" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.81</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2">
+        <v>20</v>
+      </c>
+      <c r="I3" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <v>0.88</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>17</v>
+      </c>
+      <c r="I4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>0.92</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>13</v>
+      </c>
+      <c r="I5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>0.7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>0.71</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8">
+        <v>7</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>0.43</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>0.33</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10">
+        <v>6</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2">
+        <v>4</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="2">
+        <v>5</v>
+      </c>
+      <c r="I11" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>0.5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="G18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>